<commit_message>
Add KEGG Compound Annotation, add biomass component for iMSU with KEGG ID
</commit_message>
<xml_diff>
--- a/data/biomass/Biomass_Literatures_Templates_Combined_new_correct_upload.xlsx
+++ b/data/biomass/Biomass_Literatures_Templates_Combined_new_correct_upload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gejun/Desktop/Projects/Metacardis_Gut/GEMs of species/Sharing/Microbiota-D3/data/biomass/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3721CBC7-2F3E-C44F-998B-641932209AC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD2EE4E-27FE-3C48-917B-0187E2A218CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6040" yWindow="860" windowWidth="25920" windowHeight="17800" xr2:uid="{1E65AA55-A40A-A646-A425-CDA5F7429220}"/>
+    <workbookView xWindow="340" yWindow="640" windowWidth="25920" windowHeight="17800" activeTab="2" xr2:uid="{1E65AA55-A40A-A646-A425-CDA5F7429220}"/>
   </bookViews>
   <sheets>
     <sheet name="Biomass References" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2578" uniqueCount="973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="1013">
   <si>
     <t>carveme</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -2438,9 +2438,6 @@
     <t>dTDPglucose</t>
   </si>
   <si>
-    <t>iSMU_Biomass</t>
-  </si>
-  <si>
     <t>In Silico Genome-Scale Reconstruction and</t>
   </si>
   <si>
@@ -2981,6 +2978,129 @@
   </si>
   <si>
     <t>MNXM149</t>
+  </si>
+  <si>
+    <t>iMSU_Biomass_KEGGID</t>
+  </si>
+  <si>
+    <t>iMSU_Biomass_Name</t>
+  </si>
+  <si>
+    <t>C00001</t>
+  </si>
+  <si>
+    <t>C00025</t>
+  </si>
+  <si>
+    <t>C00029</t>
+  </si>
+  <si>
+    <t>C00041</t>
+  </si>
+  <si>
+    <t>C00043</t>
+  </si>
+  <si>
+    <t>C00047</t>
+  </si>
+  <si>
+    <t>C00049</t>
+  </si>
+  <si>
+    <t>C00052</t>
+  </si>
+  <si>
+    <t>C00061</t>
+  </si>
+  <si>
+    <t>C00062</t>
+  </si>
+  <si>
+    <t>C00064</t>
+  </si>
+  <si>
+    <t>C00065</t>
+  </si>
+  <si>
+    <t>C00073</t>
+  </si>
+  <si>
+    <t>C00078</t>
+  </si>
+  <si>
+    <t>C00079</t>
+  </si>
+  <si>
+    <t>C00082</t>
+  </si>
+  <si>
+    <t>C00097</t>
+  </si>
+  <si>
+    <t>C00123</t>
+  </si>
+  <si>
+    <t>C00133</t>
+  </si>
+  <si>
+    <t>C00135</t>
+  </si>
+  <si>
+    <t>C00148</t>
+  </si>
+  <si>
+    <t>C00152</t>
+  </si>
+  <si>
+    <t>C00183</t>
+  </si>
+  <si>
+    <t>C00251</t>
+  </si>
+  <si>
+    <t>C00305</t>
+  </si>
+  <si>
+    <t>C00344</t>
+  </si>
+  <si>
+    <t>C00627</t>
+  </si>
+  <si>
+    <t>C00647</t>
+  </si>
+  <si>
+    <t>C00842</t>
+  </si>
+  <si>
+    <t>C01170</t>
+  </si>
+  <si>
+    <t>C03294</t>
+  </si>
+  <si>
+    <t>C03319</t>
+  </si>
+  <si>
+    <t>C04144</t>
+  </si>
+  <si>
+    <t>C04574</t>
+  </si>
+  <si>
+    <t>C05896(LYS)</t>
+  </si>
+  <si>
+    <t>C05980</t>
+  </si>
+  <si>
+    <t>C20897</t>
+  </si>
+  <si>
+    <t>C00009</t>
+  </si>
+  <si>
+    <t>C00035</t>
   </si>
 </sst>
 </file>
@@ -3489,7 +3609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626F503D-229B-5C42-9778-15947FDBA3F3}">
   <dimension ref="A1:CO171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -3611,10 +3731,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>837</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>838</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -3653,13 +3773,13 @@
         <v>16</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="R2" s="24" t="s">
         <v>684</v>
       </c>
       <c r="S2" s="24" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="T2" s="23" t="s">
         <v>768</v>
@@ -3878,10 +3998,10 @@
         <v>84</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>839</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>840</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>85</v>
@@ -4131,7 +4251,7 @@
         <v>92</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>85</v>
@@ -4247,10 +4367,10 @@
         <v>96</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>842</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>843</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>85</v>
@@ -4844,7 +4964,7 @@
         <v>112</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>85</v>
@@ -5197,10 +5317,10 @@
         <v>121</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>845</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>846</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>85</v>
@@ -5461,10 +5581,10 @@
         <v>121</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>845</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>846</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>85</v>
@@ -5725,10 +5845,10 @@
         <v>126</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>847</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>848</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>85</v>
@@ -5988,10 +6108,10 @@
         <v>131</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>849</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>850</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>85</v>
@@ -6365,10 +6485,10 @@
         <v>138</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>851</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>852</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>85</v>
@@ -6628,10 +6748,10 @@
         <v>142</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>853</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>854</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>85</v>
@@ -6891,10 +7011,10 @@
         <v>146</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>855</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>856</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>85</v>
@@ -7154,10 +7274,10 @@
         <v>150</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>857</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>858</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>85</v>
@@ -7421,10 +7541,10 @@
         <v>150</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>857</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>858</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>85</v>
@@ -7906,10 +8026,10 @@
         <v>159</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>859</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>860</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>85</v>
@@ -8025,10 +8145,10 @@
         <v>163</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>861</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>862</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>85</v>
@@ -8502,10 +8622,10 @@
         <v>173</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>863</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>864</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>85</v>
@@ -8874,10 +8994,10 @@
         <v>180</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>865</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>866</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>85</v>
@@ -9244,10 +9364,10 @@
         <v>187</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>867</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>868</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>85</v>
@@ -9618,10 +9738,10 @@
         <v>194</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>869</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>870</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>85</v>
@@ -9879,10 +9999,10 @@
         <v>199</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>871</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>872</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>85</v>
@@ -10136,10 +10256,10 @@
         <v>203</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>873</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>874</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>85</v>
@@ -10510,10 +10630,10 @@
         <v>210</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>875</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>876</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>85</v>
@@ -10767,10 +10887,10 @@
         <v>215</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>877</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>878</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>85</v>
@@ -11024,10 +11144,10 @@
         <v>219</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>879</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>880</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>85</v>
@@ -11757,10 +11877,10 @@
         <v>235</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>881</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>882</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>85</v>
@@ -12950,10 +13070,10 @@
         <v>263</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>883</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>884</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>85</v>
@@ -13207,10 +13327,10 @@
         <v>267</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>885</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>886</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>85</v>
@@ -13458,10 +13578,10 @@
         <v>271</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>887</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>888</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>85</v>
@@ -13948,10 +14068,10 @@
         <v>281</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>889</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>890</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>85</v>
@@ -14211,10 +14331,10 @@
         <v>285</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>891</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>892</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>85</v>
@@ -14474,10 +14594,10 @@
         <v>289</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>893</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>894</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>85</v>
@@ -15524,10 +15644,10 @@
         <v>315</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>895</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>896</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>85</v>
@@ -15791,10 +15911,10 @@
         <v>319</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>897</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>898</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>85</v>
@@ -16055,10 +16175,10 @@
         <v>324</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>899</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>900</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>85</v>
@@ -16436,10 +16556,10 @@
         <v>332</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>901</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>902</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>85</v>
@@ -16814,10 +16934,10 @@
         <v>339</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>903</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>904</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>85</v>
@@ -17077,10 +17197,10 @@
         <v>343</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>905</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>906</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>85</v>
@@ -17330,10 +17450,10 @@
         <v>347</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>907</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>908</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>348</v>
@@ -17449,10 +17569,10 @@
         <v>347</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>907</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>908</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>350</v>
@@ -17570,10 +17690,10 @@
         <v>352</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>909</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>910</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>85</v>
@@ -18277,10 +18397,10 @@
         <v>368</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>911</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>912</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>85</v>
@@ -18540,10 +18660,10 @@
         <v>372</v>
       </c>
       <c r="C84" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>913</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>914</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>85</v>
@@ -18803,10 +18923,10 @@
         <v>376</v>
       </c>
       <c r="C85" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>915</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>916</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>85</v>
@@ -19056,10 +19176,10 @@
         <v>380</v>
       </c>
       <c r="C86" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>917</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>918</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>85</v>
@@ -19185,10 +19305,10 @@
         <v>383</v>
       </c>
       <c r="C87" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>919</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>920</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>85</v>
@@ -19436,10 +19556,10 @@
         <v>387</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>921</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>922</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>85</v>
@@ -19781,7 +19901,7 @@
         <v>397</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>348</v>
@@ -19899,10 +20019,10 @@
         <v>400</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>924</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>925</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>85</v>
@@ -20281,10 +20401,10 @@
         <v>407</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>926</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>927</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>85</v>
@@ -20667,10 +20787,10 @@
         <v>414</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>928</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>929</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>85</v>
@@ -20788,10 +20908,10 @@
         <v>418</v>
       </c>
       <c r="C97" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="D97" s="1" t="s">
         <v>930</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>931</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>85</v>
@@ -20905,7 +21025,7 @@
         <v>421</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>85</v>
@@ -21023,7 +21143,7 @@
         <v>421</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>348</v>
@@ -21141,7 +21261,7 @@
         <v>424</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>85</v>
@@ -21259,7 +21379,7 @@
         <v>424</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>348</v>
@@ -21721,10 +21841,10 @@
         <v>435</v>
       </c>
       <c r="C104" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>934</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>935</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>85</v>
@@ -21984,10 +22104,10 @@
         <v>439</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>936</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>937</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>85</v>
@@ -22229,10 +22349,10 @@
         <v>444</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="D106" s="1" t="s">
         <v>938</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>939</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>85</v>
@@ -22493,10 +22613,10 @@
         <v>444</v>
       </c>
       <c r="C107" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>938</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>939</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>85</v>
@@ -22757,10 +22877,10 @@
         <v>448</v>
       </c>
       <c r="C108" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>940</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>941</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>85</v>
@@ -23016,10 +23136,10 @@
         <v>452</v>
       </c>
       <c r="C109" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>942</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>943</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>85</v>
@@ -23625,10 +23745,10 @@
         <v>464</v>
       </c>
       <c r="C112" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>944</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>945</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>85</v>
@@ -23876,10 +23996,10 @@
         <v>468</v>
       </c>
       <c r="C113" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="D113" s="1" t="s">
         <v>946</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>947</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>85</v>
@@ -24127,10 +24247,10 @@
         <v>472</v>
       </c>
       <c r="C114" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>948</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>949</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>85</v>
@@ -24390,10 +24510,10 @@
         <v>476</v>
       </c>
       <c r="C115" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>950</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>951</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>85</v>
@@ -24635,10 +24755,10 @@
         <v>481</v>
       </c>
       <c r="C116" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>952</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>953</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>85</v>
@@ -24886,10 +25006,10 @@
         <v>485</v>
       </c>
       <c r="C117" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>954</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>955</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>85</v>
@@ -25304,10 +25424,10 @@
         <v>496</v>
       </c>
       <c r="C120" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>956</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>957</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>85</v>
@@ -25566,10 +25686,10 @@
         <v>500</v>
       </c>
       <c r="C121" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>958</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>959</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>85</v>
@@ -25820,10 +25940,10 @@
         <v>505</v>
       </c>
       <c r="C122" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>960</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>961</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>85</v>
@@ -26083,10 +26203,10 @@
         <v>509</v>
       </c>
       <c r="C123" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>962</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>963</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>85</v>
@@ -26343,10 +26463,10 @@
         <v>513</v>
       </c>
       <c r="C124" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>964</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>965</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>85</v>
@@ -26717,7 +26837,7 @@
         <v>521</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>85</v>
@@ -26833,10 +26953,10 @@
         <v>524</v>
       </c>
       <c r="C127" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="D127" s="1" t="s">
         <v>967</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>968</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>85</v>
@@ -27096,10 +27216,10 @@
         <v>528</v>
       </c>
       <c r="C128" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>969</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>970</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>85</v>
@@ -27359,10 +27479,10 @@
         <v>532</v>
       </c>
       <c r="C129" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="D129" s="1" t="s">
         <v>971</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>972</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>85</v>
@@ -34786,13 +34906,13 @@
         <v>735</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="K1" s="16" t="s">
         <v>4</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="M1" s="16" t="s">
         <v>771</v>
@@ -34806,10 +34926,10 @@
         <v>736</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="K2" s="16" t="s">
         <v>84</v>
@@ -34823,10 +34943,10 @@
         <v>737</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>92</v>
@@ -34840,7 +34960,7 @@
         <v>738</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>96</v>
@@ -34854,7 +34974,7 @@
         <v>739</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>99</v>
@@ -34874,7 +34994,7 @@
         <v>740</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>103</v>
@@ -34894,7 +35014,7 @@
         <v>741</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>106</v>
@@ -34914,7 +35034,7 @@
         <v>742</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K8" s="16" t="s">
         <v>109</v>
@@ -34934,7 +35054,7 @@
         <v>289</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>112</v>
@@ -34948,7 +35068,7 @@
         <v>743</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>115</v>
@@ -34968,7 +35088,7 @@
         <v>744</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>118</v>
@@ -34988,7 +35108,7 @@
         <v>745</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>121</v>
@@ -35008,7 +35128,7 @@
         <v>746</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>121</v>
@@ -35028,13 +35148,13 @@
         <v>747</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="M14">
         <v>0.56210000000000004</v>
@@ -35048,7 +35168,7 @@
         <v>748</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K15" s="16" t="s">
         <v>131</v>
@@ -35062,7 +35182,7 @@
         <v>749</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>135</v>
@@ -35082,13 +35202,13 @@
         <v>750</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="M17">
         <v>0.32369999999999999</v>
@@ -35102,13 +35222,13 @@
         <v>751</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="M18">
         <v>0.26379999999999998</v>
@@ -35122,13 +35242,13 @@
         <v>752</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="M19">
         <v>0.26379999999999998</v>
@@ -35142,7 +35262,7 @@
         <v>753</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K20" s="16" t="s">
         <v>150</v>
@@ -35162,7 +35282,7 @@
         <v>754</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>150</v>
@@ -35182,7 +35302,7 @@
         <v>459</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>154</v>
@@ -35196,7 +35316,7 @@
         <v>336</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>159</v>
@@ -35391,10 +35511,10 @@
         <v>540</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="L35" s="16" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="M35">
         <v>0.1002</v>
@@ -35408,7 +35528,7 @@
         <v>135</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K36" s="16" t="s">
         <v>207</v>
@@ -35841,10 +35961,10 @@
         <v>87</v>
       </c>
       <c r="K59" s="16" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="L59" s="16" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="M59">
         <v>0.28799999999999998</v>
@@ -35861,10 +35981,10 @@
         <v>87</v>
       </c>
       <c r="K60" s="16" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="L60" s="16" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="M60">
         <v>0.28799999999999998</v>
@@ -35912,13 +36032,13 @@
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="14" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B63" s="12" t="s">
         <v>150</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="K63" s="16" t="s">
         <v>297</v>
@@ -35932,7 +36052,7 @@
         <v>324</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="K64" s="16" t="s">
         <v>300</v>
@@ -35948,13 +36068,13 @@
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="14" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B66" s="12" t="s">
         <v>121</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="K66" s="16" t="s">
         <v>311</v>
@@ -35968,7 +36088,7 @@
         <v>319</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="K67" s="16" t="s">
         <v>315</v>
@@ -35988,7 +36108,7 @@
         <v>444</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="K68" s="16" t="s">
         <v>319</v>
@@ -36008,7 +36128,7 @@
         <v>448</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="K69" s="16" t="s">
         <v>324</v>
@@ -36033,10 +36153,10 @@
     </row>
     <row r="71" spans="1:13">
       <c r="K71" s="16" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="L71" s="16" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="M71">
         <v>0.1037</v>
@@ -36058,10 +36178,10 @@
     </row>
     <row r="73" spans="1:13">
       <c r="K73" s="16" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="L73" s="16" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="M73">
         <v>0.31790000000000002</v>
@@ -36084,10 +36204,10 @@
     </row>
     <row r="77" spans="1:13">
       <c r="K77" s="16" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="L77" s="16" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="M77">
         <v>0.49299999999999999</v>
@@ -36115,10 +36235,10 @@
     </row>
     <row r="82" spans="11:13">
       <c r="K82" s="16" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="L82" s="16" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="M82">
         <v>0.3755</v>
@@ -36126,10 +36246,10 @@
     </row>
     <row r="83" spans="11:13">
       <c r="K83" s="16" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="L83" s="16" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="M83">
         <v>0.16819999999999999</v>
@@ -36256,10 +36376,10 @@
     </row>
     <row r="103" spans="11:13">
       <c r="K103" s="16" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="L103" s="16" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="M103">
         <v>0.20269999999999999</v>
@@ -36305,10 +36425,10 @@
     </row>
     <row r="108" spans="11:13">
       <c r="K108" s="16" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="L108" s="16" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="M108">
         <v>0.2419</v>
@@ -36342,10 +36462,10 @@
     </row>
     <row r="113" spans="11:13">
       <c r="K113" s="16" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="L113" s="16" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="M113">
         <v>0.2361</v>
@@ -36400,10 +36520,10 @@
     </row>
     <row r="121" spans="11:13">
       <c r="K121" s="16" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="L121" s="16" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="M121">
         <v>0.27760000000000001</v>
@@ -36411,10 +36531,10 @@
     </row>
     <row r="122" spans="11:13">
       <c r="K122" s="16" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="L122" s="16" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="M122">
         <v>6.2199999999999998E-2</v>
@@ -36422,10 +36542,10 @@
     </row>
     <row r="123" spans="11:13">
       <c r="K123" s="16" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="L123" s="16" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="M123">
         <v>0.15090000000000001</v>
@@ -36454,10 +36574,10 @@
     </row>
     <row r="127" spans="11:13">
       <c r="K127" s="16" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="L127" s="16" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="M127">
         <v>0.46310000000000001</v>
@@ -36475,894 +36595,1082 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F103645-002D-5644-B2A8-73FF429E7500}">
-  <dimension ref="B1:L151"/>
+  <dimension ref="A1:J151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="32.6640625" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="6" max="10" width="12.1640625" customWidth="1"/>
-    <col min="11" max="11" width="32.6640625" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" customWidth="1"/>
+    <col min="3" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="8" width="12.1640625" customWidth="1"/>
+    <col min="9" max="9" width="32.6640625" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12">
+    <row r="1" spans="1:10">
+      <c r="A1" s="16" t="s">
+        <v>972</v>
+      </c>
       <c r="B1" s="16" t="s">
-        <v>792</v>
+        <v>973</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>771</v>
       </c>
+      <c r="D1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-    </row>
-    <row r="2" spans="2:12" ht="23">
+    </row>
+    <row r="2" spans="1:10" ht="23">
+      <c r="A2" s="16" t="s">
+        <v>974</v>
+      </c>
       <c r="B2" s="16" t="s">
-        <v>122</v>
+        <v>325</v>
       </c>
       <c r="C2">
         <v>33.128999999999998</v>
       </c>
-      <c r="G2" s="19" t="s">
-        <v>800</v>
-      </c>
-      <c r="J2" s="16"/>
-    </row>
-    <row r="3" spans="2:12" ht="23">
+      <c r="E2" s="19" t="s">
+        <v>799</v>
+      </c>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:10" ht="23">
+      <c r="A3" s="16" t="s">
+        <v>856</v>
+      </c>
       <c r="B3" s="16" t="s">
         <v>151</v>
       </c>
       <c r="C3">
         <v>28.329000000000001</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>801</v>
-      </c>
-      <c r="J3" s="16"/>
-    </row>
-    <row r="4" spans="2:12">
+      <c r="E3" s="19" t="s">
+        <v>800</v>
+      </c>
+      <c r="H3" s="16"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="16" t="s">
+        <v>923</v>
+      </c>
       <c r="B4" s="16" t="s">
-        <v>772</v>
+        <v>401</v>
       </c>
       <c r="C4">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="2:12">
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="16" t="s">
+        <v>925</v>
+      </c>
       <c r="B5" s="16" t="s">
-        <v>195</v>
+        <v>408</v>
       </c>
       <c r="C5">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="2:12">
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="16" t="s">
+        <v>864</v>
+      </c>
       <c r="B6" s="16" t="s">
-        <v>714</v>
+        <v>725</v>
       </c>
       <c r="C6">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="J6" s="16"/>
-    </row>
-    <row r="7" spans="2:12">
+      <c r="H6" s="16"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="16" t="s">
+        <v>882</v>
+      </c>
       <c r="B7" s="16" t="s">
-        <v>773</v>
+        <v>264</v>
       </c>
       <c r="C7">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J7" s="16"/>
-    </row>
-    <row r="8" spans="2:12">
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="16" t="s">
+        <v>943</v>
+      </c>
       <c r="B8" s="16" t="s">
-        <v>725</v>
+        <v>781</v>
       </c>
       <c r="C8">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="2:12">
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="16" t="s">
+        <v>848</v>
+      </c>
       <c r="B9" s="16" t="s">
-        <v>774</v>
+        <v>132</v>
       </c>
       <c r="C9">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="2:12">
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="16" t="s">
+        <v>975</v>
+      </c>
       <c r="B10" s="16" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="C10">
         <v>0.155</v>
       </c>
-      <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="2:12">
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="16" t="s">
+        <v>976</v>
+      </c>
       <c r="B11" s="16" t="s">
-        <v>775</v>
+        <v>789</v>
       </c>
       <c r="C11">
         <v>0.75800000000000001</v>
       </c>
-      <c r="J11" s="16"/>
-    </row>
-    <row r="12" spans="2:12">
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="16" t="s">
+        <v>892</v>
+      </c>
       <c r="B12" s="16" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="C12">
         <v>0.152</v>
       </c>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="2:12">
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="16" t="s">
+        <v>977</v>
+      </c>
       <c r="B13" s="16" t="s">
-        <v>316</v>
+        <v>127</v>
       </c>
       <c r="C13">
         <v>0.18099999999999999</v>
       </c>
-      <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="2:12">
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="16" t="s">
+        <v>978</v>
+      </c>
       <c r="B14" s="16" t="s">
-        <v>776</v>
+        <v>787</v>
       </c>
       <c r="C14">
         <v>0.29299999999999998</v>
       </c>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="15" spans="2:12">
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="16" t="s">
+        <v>894</v>
+      </c>
       <c r="B15" s="16" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
       <c r="C15">
         <v>4.9180000000000001</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-    </row>
-    <row r="16" spans="2:12">
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="16" t="s">
+        <v>979</v>
+      </c>
       <c r="B16" s="16" t="s">
-        <v>320</v>
+        <v>369</v>
       </c>
       <c r="C16">
         <v>0.18</v>
       </c>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-    </row>
-    <row r="17" spans="2:11">
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="16" t="s">
+        <v>980</v>
+      </c>
       <c r="B17" s="16" t="s">
-        <v>325</v>
+        <v>147</v>
       </c>
       <c r="C17">
         <v>0.13700000000000001</v>
       </c>
-      <c r="J17" s="16"/>
-    </row>
-    <row r="18" spans="2:11">
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="16" t="s">
+        <v>981</v>
+      </c>
       <c r="B18" s="16" t="s">
-        <v>127</v>
+        <v>788</v>
       </c>
       <c r="C18">
         <v>0.129</v>
       </c>
-      <c r="J18" s="16"/>
-    </row>
-    <row r="19" spans="2:11">
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="16" t="s">
+        <v>982</v>
+      </c>
       <c r="B19" s="16" t="s">
-        <v>139</v>
+        <v>775</v>
       </c>
       <c r="C19">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-    </row>
-    <row r="20" spans="2:11">
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="16" t="s">
+        <v>983</v>
+      </c>
       <c r="B20" s="16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C20">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-    </row>
-    <row r="21" spans="2:11">
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="16" t="s">
+        <v>868</v>
+      </c>
       <c r="B21" s="16" t="s">
-        <v>147</v>
+        <v>195</v>
       </c>
       <c r="C21">
         <v>4.7E-2</v>
       </c>
-      <c r="K21" s="16"/>
-    </row>
-    <row r="22" spans="2:11">
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="16" t="s">
+        <v>984</v>
+      </c>
       <c r="B22" s="16" t="s">
-        <v>204</v>
+        <v>282</v>
       </c>
       <c r="C22">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="J22" s="16"/>
-    </row>
-    <row r="23" spans="2:11">
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="16" t="s">
+        <v>985</v>
+      </c>
       <c r="B23" s="16" t="s">
-        <v>286</v>
+        <v>473</v>
       </c>
       <c r="C23">
         <v>0.153</v>
       </c>
-      <c r="J23" s="16"/>
-    </row>
-    <row r="24" spans="2:11">
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="16" t="s">
+        <v>957</v>
+      </c>
       <c r="B24" s="16" t="s">
-        <v>282</v>
+        <v>501</v>
       </c>
       <c r="C24">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J24" s="16"/>
-    </row>
-    <row r="25" spans="2:11">
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="16" t="s">
+        <v>986</v>
+      </c>
       <c r="B25" s="16" t="s">
-        <v>333</v>
+        <v>373</v>
       </c>
       <c r="C25">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="K25" s="16"/>
-    </row>
-    <row r="26" spans="2:11">
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="16" t="s">
+        <v>966</v>
+      </c>
       <c r="B26" s="16" t="s">
-        <v>340</v>
+        <v>525</v>
       </c>
       <c r="C26">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="J26" s="16"/>
-    </row>
-    <row r="27" spans="2:11">
+      <c r="H26" s="16"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="16" t="s">
+        <v>987</v>
+      </c>
       <c r="B27" s="16" t="s">
-        <v>353</v>
+        <v>510</v>
       </c>
       <c r="C27">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="J27" s="16"/>
-    </row>
-    <row r="28" spans="2:11">
+      <c r="H27" s="16"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="16" t="s">
+        <v>988</v>
+      </c>
       <c r="B28" s="16" t="s">
-        <v>369</v>
+        <v>436</v>
       </c>
       <c r="C28">
         <v>0.11600000000000001</v>
       </c>
-      <c r="J28" s="16"/>
-    </row>
-    <row r="29" spans="2:11">
+      <c r="H28" s="16"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="16" t="s">
+        <v>989</v>
+      </c>
       <c r="B29" s="16" t="s">
-        <v>373</v>
+        <v>514</v>
       </c>
       <c r="C29">
         <v>9.4E-2</v>
       </c>
-      <c r="K29" s="16"/>
-    </row>
-    <row r="30" spans="2:11">
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="16" t="s">
+        <v>990</v>
+      </c>
       <c r="B30" s="16" t="s">
-        <v>436</v>
+        <v>204</v>
       </c>
       <c r="C30">
         <v>1.4E-2</v>
       </c>
-      <c r="J30" s="16"/>
-    </row>
-    <row r="31" spans="2:11">
+      <c r="H30" s="16"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="16" t="s">
+        <v>955</v>
+      </c>
       <c r="B31" s="16" t="s">
-        <v>453</v>
+        <v>497</v>
       </c>
       <c r="C31">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J31" s="16"/>
-    </row>
-    <row r="32" spans="2:11">
+      <c r="H31" s="16"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="16" t="s">
+        <v>991</v>
+      </c>
       <c r="B32" s="16" t="s">
-        <v>473</v>
+        <v>353</v>
       </c>
       <c r="C32">
         <v>0.246</v>
       </c>
-      <c r="K32" s="16"/>
-    </row>
-    <row r="33" spans="2:11">
+      <c r="I32" s="16"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="16" t="s">
+        <v>874</v>
+      </c>
       <c r="B33" s="16" t="s">
-        <v>506</v>
+        <v>707</v>
       </c>
       <c r="C33">
         <v>1.9E-2</v>
       </c>
-      <c r="J33" s="16"/>
-    </row>
-    <row r="34" spans="2:11">
+      <c r="H33" s="16"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="16" t="s">
+        <v>992</v>
+      </c>
       <c r="B34" s="16" t="s">
-        <v>510</v>
+        <v>774</v>
       </c>
       <c r="C34">
         <v>0.158</v>
       </c>
-      <c r="J34" s="16"/>
-    </row>
-    <row r="35" spans="2:11">
+      <c r="H34" s="16"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="16" t="s">
+        <v>993</v>
+      </c>
       <c r="B35" s="16" t="s">
-        <v>514</v>
+        <v>333</v>
       </c>
       <c r="C35">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="J35" s="16"/>
-    </row>
-    <row r="36" spans="2:11">
+      <c r="H35" s="16"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="16" t="s">
+        <v>994</v>
+      </c>
       <c r="B36" s="16" t="s">
-        <v>529</v>
+        <v>453</v>
       </c>
       <c r="C36">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="J36" s="16"/>
-    </row>
-    <row r="37" spans="2:11">
+      <c r="H36" s="16"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="16" t="s">
+        <v>995</v>
+      </c>
       <c r="B37" s="16" t="s">
-        <v>777</v>
+        <v>143</v>
       </c>
       <c r="C37">
         <v>0.11799999999999999</v>
       </c>
-      <c r="J37" s="16"/>
-    </row>
-    <row r="38" spans="2:11">
+      <c r="H37" s="16"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="16" t="s">
+        <v>996</v>
+      </c>
       <c r="B38" s="16" t="s">
-        <v>778</v>
+        <v>529</v>
       </c>
       <c r="C38">
         <v>0.16</v>
       </c>
-      <c r="J38" s="16"/>
-    </row>
-    <row r="39" spans="2:11">
+      <c r="H38" s="16"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="16" t="s">
+        <v>959</v>
+      </c>
       <c r="B39" s="16" t="s">
-        <v>779</v>
+        <v>506</v>
       </c>
       <c r="C39">
         <v>0.13600000000000001</v>
       </c>
-      <c r="J39" s="16"/>
-    </row>
-    <row r="40" spans="2:11">
+      <c r="H39" s="16"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="16" t="s">
+        <v>997</v>
+      </c>
       <c r="B40" s="16" t="s">
-        <v>401</v>
+        <v>773</v>
       </c>
       <c r="C40">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="J40" s="16"/>
-    </row>
-    <row r="41" spans="2:11">
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="16" t="s">
+        <v>878</v>
+      </c>
       <c r="B41" s="16" t="s">
-        <v>408</v>
+        <v>709</v>
       </c>
       <c r="C41">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="J41" s="16"/>
-    </row>
-    <row r="42" spans="2:11">
+      <c r="H41" s="16"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="16" t="s">
+        <v>998</v>
+      </c>
       <c r="B42" s="16" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C42">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J42" s="16"/>
-    </row>
-    <row r="43" spans="2:11">
+      <c r="H42" s="16"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="16" t="s">
+        <v>999</v>
+      </c>
       <c r="B43" s="16" t="s">
-        <v>445</v>
+        <v>713</v>
       </c>
       <c r="C43">
         <v>7.9000000000000001E-4</v>
       </c>
-      <c r="J43" s="16"/>
-    </row>
-    <row r="44" spans="2:11">
+      <c r="H43" s="16"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="16" t="s">
+        <v>902</v>
+      </c>
       <c r="B44" s="16" t="s">
-        <v>713</v>
+        <v>340</v>
       </c>
       <c r="C44">
         <v>0.188</v>
       </c>
-      <c r="J44" s="16"/>
-    </row>
-    <row r="45" spans="2:11">
+      <c r="H44" s="16"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="16" t="s">
+        <v>876</v>
+      </c>
       <c r="B45" s="16" t="s">
-        <v>781</v>
+        <v>708</v>
       </c>
       <c r="C45">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="J45" s="16"/>
-      <c r="K45" s="16"/>
-    </row>
-    <row r="46" spans="2:11">
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="16" t="s">
+        <v>880</v>
+      </c>
       <c r="B46" s="16" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="C46">
         <v>1.9E-2</v>
       </c>
-      <c r="J46" s="16"/>
-    </row>
-    <row r="47" spans="2:11">
+      <c r="H46" s="16"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="16" t="s">
+        <v>1000</v>
+      </c>
       <c r="B47" s="16" t="s">
         <v>783</v>
       </c>
       <c r="C47">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="K47" s="16"/>
-    </row>
-    <row r="48" spans="2:11">
+      <c r="I47" s="16"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="16" t="s">
+        <v>1001</v>
+      </c>
       <c r="B48" s="16" t="s">
-        <v>132</v>
+        <v>782</v>
       </c>
       <c r="C48">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J48" s="16"/>
-      <c r="K48" s="16"/>
-    </row>
-    <row r="49" spans="2:11">
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="16" t="s">
+        <v>1002</v>
+      </c>
       <c r="B49" s="16" t="s">
-        <v>784</v>
+        <v>791</v>
       </c>
       <c r="C49">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="J49" s="16"/>
-      <c r="K49" s="16"/>
-    </row>
-    <row r="50" spans="2:11">
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="16" t="s">
+        <v>1003</v>
+      </c>
       <c r="B50" s="16" t="s">
-        <v>497</v>
+        <v>786</v>
       </c>
       <c r="C50">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="J50" s="16"/>
-      <c r="K50" s="16"/>
-    </row>
-    <row r="51" spans="2:11">
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="16" t="s">
+        <v>1004</v>
+      </c>
       <c r="B51" s="16" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="C51">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="J51" s="16"/>
-    </row>
-    <row r="52" spans="2:11">
+      <c r="H51" s="16"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="16" t="s">
+        <v>1005</v>
+      </c>
       <c r="B52" s="16" t="s">
-        <v>501</v>
+        <v>790</v>
       </c>
       <c r="C52">
         <v>0.17199999999999999</v>
       </c>
-      <c r="J52" s="16"/>
-    </row>
-    <row r="53" spans="2:11">
+      <c r="H52" s="16"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="16" t="s">
+        <v>1006</v>
+      </c>
       <c r="B53" s="16" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C53">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="K53" s="16"/>
-    </row>
-    <row r="54" spans="2:11">
+      <c r="I53" s="16"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="16" t="s">
+        <v>1007</v>
+      </c>
       <c r="B54" s="16" t="s">
-        <v>787</v>
+        <v>772</v>
       </c>
       <c r="C54">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="K54" s="16"/>
-    </row>
-    <row r="55" spans="2:11">
+      <c r="I54" s="16"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="16" t="s">
+        <v>1008</v>
+      </c>
       <c r="B55" s="16" t="s">
-        <v>788</v>
+        <v>777</v>
       </c>
       <c r="C55">
         <v>0.14599999999999999</v>
       </c>
-      <c r="J55" s="16"/>
-    </row>
-    <row r="56" spans="2:11">
+      <c r="H55" s="16"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="16" t="s">
+        <v>1009</v>
+      </c>
       <c r="B56" s="16" t="s">
-        <v>789</v>
+        <v>714</v>
       </c>
       <c r="C56">
         <v>1.8E-5</v>
       </c>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16"/>
-    </row>
-    <row r="57" spans="2:11">
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="16" t="s">
+        <v>1010</v>
+      </c>
       <c r="B57" s="16" t="s">
-        <v>525</v>
+        <v>776</v>
       </c>
       <c r="C57">
         <v>1.2999999999999999E-4</v>
       </c>
-      <c r="J57" s="16"/>
-    </row>
-    <row r="58" spans="2:11">
+      <c r="H57" s="16"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="16" t="s">
+        <v>844</v>
+      </c>
       <c r="B58" s="16" t="s">
-        <v>707</v>
+        <v>122</v>
       </c>
       <c r="C58">
         <v>28.242000000000001</v>
       </c>
-      <c r="J58" s="16"/>
-    </row>
-    <row r="59" spans="2:11">
+      <c r="H58" s="16"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="16" t="s">
+        <v>1011</v>
+      </c>
       <c r="B59" s="16" t="s">
-        <v>708</v>
+        <v>445</v>
       </c>
       <c r="C59">
         <v>33.1</v>
       </c>
-      <c r="K59" s="16"/>
-    </row>
-    <row r="60" spans="2:11">
+      <c r="I59" s="16"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="16" t="s">
+        <v>939</v>
+      </c>
       <c r="B60" s="16" t="s">
-        <v>709</v>
+        <v>780</v>
       </c>
       <c r="C60">
         <v>0.34010000000000001</v>
       </c>
-      <c r="J60" s="16"/>
-      <c r="K60" s="16"/>
-    </row>
-    <row r="61" spans="2:11">
+      <c r="H60" s="16"/>
+      <c r="I60" s="16"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="16" t="s">
+        <v>1012</v>
+      </c>
       <c r="B61" s="16" t="s">
-        <v>790</v>
+        <v>276</v>
       </c>
       <c r="C61">
         <v>4.8600000000000003</v>
       </c>
-      <c r="J61" s="16"/>
-    </row>
-    <row r="62" spans="2:11">
+      <c r="H61" s="16"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="16" t="s">
+        <v>896</v>
+      </c>
       <c r="B62" s="16" t="s">
-        <v>791</v>
+        <v>320</v>
       </c>
       <c r="C62">
         <v>33.1</v>
       </c>
-      <c r="J62" s="16"/>
-    </row>
-    <row r="63" spans="2:11">
-      <c r="J63" s="16"/>
-    </row>
-    <row r="64" spans="2:11">
-      <c r="J64" s="16"/>
-    </row>
-    <row r="65" spans="10:11">
-      <c r="K65" s="16"/>
-    </row>
-    <row r="66" spans="10:11">
-      <c r="J66" s="16"/>
-      <c r="K66" s="16"/>
-    </row>
-    <row r="67" spans="10:11">
-      <c r="J67" s="16"/>
-    </row>
-    <row r="68" spans="10:11">
-      <c r="J68" s="16"/>
-    </row>
-    <row r="69" spans="10:11">
-      <c r="J69" s="16"/>
-      <c r="K69" s="16"/>
-    </row>
-    <row r="70" spans="10:11">
-      <c r="J70" s="16"/>
-      <c r="K70" s="16"/>
-    </row>
-    <row r="71" spans="10:11">
-      <c r="J71" s="16"/>
-      <c r="K71" s="16"/>
-    </row>
-    <row r="72" spans="10:11">
-      <c r="J72" s="16"/>
-    </row>
-    <row r="73" spans="10:11">
-      <c r="J73" s="16"/>
-    </row>
-    <row r="74" spans="10:11">
-      <c r="J74" s="16"/>
-      <c r="K74" s="16"/>
-    </row>
-    <row r="75" spans="10:11">
-      <c r="J75" s="16"/>
-      <c r="K75" s="16"/>
-    </row>
-    <row r="76" spans="10:11">
-      <c r="J76" s="16"/>
-      <c r="K76" s="16"/>
-    </row>
-    <row r="77" spans="10:11">
-      <c r="J77" s="16"/>
-      <c r="K77" s="16"/>
-    </row>
-    <row r="78" spans="10:11">
-      <c r="J78" s="16"/>
-      <c r="K78" s="16"/>
-    </row>
-    <row r="79" spans="10:11">
-      <c r="J79" s="16"/>
-      <c r="K79" s="16"/>
-    </row>
-    <row r="80" spans="10:11">
-      <c r="J80" s="16"/>
-      <c r="K80" s="16"/>
-    </row>
-    <row r="81" spans="10:11">
-      <c r="J81" s="16"/>
-      <c r="K81" s="16"/>
-    </row>
-    <row r="82" spans="10:11">
-      <c r="J82" s="16"/>
-      <c r="K82" s="16"/>
-    </row>
-    <row r="83" spans="10:11">
-      <c r="J83" s="16"/>
-      <c r="K83" s="16"/>
-    </row>
-    <row r="84" spans="10:11">
-      <c r="J84" s="16"/>
-      <c r="K84" s="16"/>
-    </row>
-    <row r="85" spans="10:11">
-      <c r="J85" s="16"/>
-      <c r="K85" s="16"/>
-    </row>
-    <row r="86" spans="10:11">
-      <c r="J86" s="16"/>
-      <c r="K86" s="16"/>
-    </row>
-    <row r="87" spans="10:11">
-      <c r="J87" s="16"/>
-      <c r="K87" s="16"/>
-    </row>
-    <row r="88" spans="10:11">
-      <c r="J88" s="16"/>
-      <c r="K88" s="16"/>
-    </row>
-    <row r="89" spans="10:11">
-      <c r="J89" s="16"/>
-      <c r="K89" s="16"/>
-    </row>
-    <row r="90" spans="10:11">
-      <c r="J90" s="16"/>
-      <c r="K90" s="16"/>
-    </row>
-    <row r="91" spans="10:11">
-      <c r="J91" s="16"/>
-      <c r="K91" s="16"/>
-    </row>
-    <row r="92" spans="10:11">
-      <c r="J92" s="16"/>
-      <c r="K92" s="16"/>
-    </row>
-    <row r="93" spans="10:11">
-      <c r="J93" s="16"/>
-    </row>
-    <row r="94" spans="10:11">
-      <c r="J94" s="16"/>
-    </row>
-    <row r="95" spans="10:11">
-      <c r="J95" s="16"/>
-    </row>
-    <row r="96" spans="10:11">
-      <c r="J96" s="16"/>
-    </row>
-    <row r="97" spans="10:11">
-      <c r="K97" s="16"/>
-    </row>
-    <row r="98" spans="10:11">
-      <c r="J98" s="16"/>
-    </row>
-    <row r="99" spans="10:11">
-      <c r="J99" s="16"/>
-    </row>
-    <row r="100" spans="10:11">
-      <c r="J100" s="16"/>
-    </row>
-    <row r="101" spans="10:11">
-      <c r="K101" s="16"/>
-    </row>
-    <row r="102" spans="10:11">
-      <c r="J102" s="16"/>
-    </row>
-    <row r="103" spans="10:11">
-      <c r="J103" s="16"/>
-    </row>
-    <row r="104" spans="10:11">
-      <c r="J104" s="16"/>
-    </row>
-    <row r="105" spans="10:11">
-      <c r="K105" s="16"/>
-    </row>
-    <row r="106" spans="10:11">
-      <c r="J106" s="16"/>
-      <c r="K106" s="16"/>
-    </row>
-    <row r="107" spans="10:11">
-      <c r="J107" s="16"/>
-      <c r="K107" s="16"/>
-    </row>
-    <row r="108" spans="10:11">
-      <c r="J108" s="16"/>
-    </row>
-    <row r="109" spans="10:11">
-      <c r="J109" s="16"/>
-    </row>
-    <row r="110" spans="10:11">
-      <c r="J110" s="16"/>
-    </row>
-    <row r="111" spans="10:11">
-      <c r="J111" s="16"/>
-    </row>
-    <row r="112" spans="10:11">
-      <c r="J112" s="16"/>
-      <c r="K112" s="16"/>
-    </row>
-    <row r="113" spans="10:11">
-      <c r="J113" s="16"/>
-      <c r="K113" s="16"/>
-    </row>
-    <row r="114" spans="10:11">
-      <c r="J114" s="16"/>
-    </row>
-    <row r="115" spans="10:11">
-      <c r="J115" s="16"/>
-    </row>
-    <row r="116" spans="10:11">
-      <c r="J116" s="16"/>
-    </row>
-    <row r="117" spans="10:11">
-      <c r="J117" s="16"/>
-    </row>
-    <row r="118" spans="10:11">
-      <c r="J118" s="16"/>
-    </row>
-    <row r="119" spans="10:11">
-      <c r="K119" s="16"/>
-    </row>
-    <row r="120" spans="10:11">
-      <c r="J120" s="16"/>
-    </row>
-    <row r="121" spans="10:11">
-      <c r="J121" s="16"/>
-    </row>
-    <row r="122" spans="10:11">
-      <c r="K122" s="16"/>
-    </row>
-    <row r="123" spans="10:11">
-      <c r="J123" s="16"/>
-    </row>
-    <row r="124" spans="10:11">
-      <c r="J124" s="16"/>
-    </row>
-    <row r="125" spans="10:11">
-      <c r="J125" s="16"/>
-    </row>
-    <row r="126" spans="10:11">
-      <c r="K126" s="16"/>
-    </row>
-    <row r="127" spans="10:11">
-      <c r="K127" s="16"/>
-    </row>
-    <row r="128" spans="10:11">
-      <c r="K128" s="16"/>
-    </row>
-    <row r="129" spans="10:11">
-      <c r="J129" s="16"/>
-    </row>
-    <row r="130" spans="10:11">
-      <c r="J130" s="16"/>
-      <c r="K130" s="16"/>
-    </row>
-    <row r="131" spans="10:11">
-      <c r="J131" s="16"/>
-    </row>
-    <row r="132" spans="10:11">
-      <c r="J132" s="16"/>
-    </row>
-    <row r="133" spans="10:11">
-      <c r="J133" s="16"/>
-    </row>
-    <row r="134" spans="10:11">
-      <c r="J134" s="16"/>
-    </row>
-    <row r="135" spans="10:11">
-      <c r="J135" s="16"/>
-      <c r="K135" s="16"/>
-    </row>
-    <row r="136" spans="10:11">
-      <c r="K136" s="16"/>
-    </row>
-    <row r="137" spans="10:11">
-      <c r="J137" s="16"/>
-    </row>
-    <row r="138" spans="10:11">
-      <c r="J138" s="16"/>
-      <c r="K138" s="16"/>
-    </row>
-    <row r="139" spans="10:11">
-      <c r="J139" s="16"/>
-    </row>
-    <row r="140" spans="10:11">
-      <c r="K140" s="16"/>
-    </row>
-    <row r="141" spans="10:11">
-      <c r="J141" s="16"/>
-    </row>
-    <row r="142" spans="10:11">
-      <c r="K142" s="16"/>
-    </row>
-    <row r="143" spans="10:11">
-      <c r="K143" s="16"/>
-    </row>
-    <row r="144" spans="10:11">
-      <c r="K144" s="16"/>
-    </row>
-    <row r="145" spans="10:11">
-      <c r="K145" s="16"/>
-    </row>
-    <row r="146" spans="10:11">
-      <c r="J146" s="16"/>
-    </row>
-    <row r="147" spans="10:11">
-      <c r="J147" s="16"/>
-    </row>
-    <row r="148" spans="10:11">
-      <c r="J148" s="16"/>
-      <c r="K148" s="16"/>
-    </row>
-    <row r="149" spans="10:11">
-      <c r="J149" s="16"/>
-    </row>
-    <row r="150" spans="10:11">
-      <c r="J150" s="16"/>
-    </row>
-    <row r="151" spans="10:11">
-      <c r="J151" s="16"/>
+      <c r="H62" s="16"/>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="H63" s="16"/>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="H64" s="16"/>
+    </row>
+    <row r="65" spans="8:9">
+      <c r="I65" s="16"/>
+    </row>
+    <row r="66" spans="8:9">
+      <c r="H66" s="16"/>
+      <c r="I66" s="16"/>
+    </row>
+    <row r="67" spans="8:9">
+      <c r="H67" s="16"/>
+    </row>
+    <row r="68" spans="8:9">
+      <c r="H68" s="16"/>
+    </row>
+    <row r="69" spans="8:9">
+      <c r="H69" s="16"/>
+      <c r="I69" s="16"/>
+    </row>
+    <row r="70" spans="8:9">
+      <c r="H70" s="16"/>
+      <c r="I70" s="16"/>
+    </row>
+    <row r="71" spans="8:9">
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
+    </row>
+    <row r="72" spans="8:9">
+      <c r="H72" s="16"/>
+    </row>
+    <row r="73" spans="8:9">
+      <c r="H73" s="16"/>
+    </row>
+    <row r="74" spans="8:9">
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+    </row>
+    <row r="75" spans="8:9">
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
+    </row>
+    <row r="76" spans="8:9">
+      <c r="H76" s="16"/>
+      <c r="I76" s="16"/>
+    </row>
+    <row r="77" spans="8:9">
+      <c r="H77" s="16"/>
+      <c r="I77" s="16"/>
+    </row>
+    <row r="78" spans="8:9">
+      <c r="H78" s="16"/>
+      <c r="I78" s="16"/>
+    </row>
+    <row r="79" spans="8:9">
+      <c r="H79" s="16"/>
+      <c r="I79" s="16"/>
+    </row>
+    <row r="80" spans="8:9">
+      <c r="H80" s="16"/>
+      <c r="I80" s="16"/>
+    </row>
+    <row r="81" spans="8:9">
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
+    </row>
+    <row r="82" spans="8:9">
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+    </row>
+    <row r="83" spans="8:9">
+      <c r="H83" s="16"/>
+      <c r="I83" s="16"/>
+    </row>
+    <row r="84" spans="8:9">
+      <c r="H84" s="16"/>
+      <c r="I84" s="16"/>
+    </row>
+    <row r="85" spans="8:9">
+      <c r="H85" s="16"/>
+      <c r="I85" s="16"/>
+    </row>
+    <row r="86" spans="8:9">
+      <c r="H86" s="16"/>
+      <c r="I86" s="16"/>
+    </row>
+    <row r="87" spans="8:9">
+      <c r="H87" s="16"/>
+      <c r="I87" s="16"/>
+    </row>
+    <row r="88" spans="8:9">
+      <c r="H88" s="16"/>
+      <c r="I88" s="16"/>
+    </row>
+    <row r="89" spans="8:9">
+      <c r="H89" s="16"/>
+      <c r="I89" s="16"/>
+    </row>
+    <row r="90" spans="8:9">
+      <c r="H90" s="16"/>
+      <c r="I90" s="16"/>
+    </row>
+    <row r="91" spans="8:9">
+      <c r="H91" s="16"/>
+      <c r="I91" s="16"/>
+    </row>
+    <row r="92" spans="8:9">
+      <c r="H92" s="16"/>
+      <c r="I92" s="16"/>
+    </row>
+    <row r="93" spans="8:9">
+      <c r="H93" s="16"/>
+    </row>
+    <row r="94" spans="8:9">
+      <c r="H94" s="16"/>
+    </row>
+    <row r="95" spans="8:9">
+      <c r="H95" s="16"/>
+    </row>
+    <row r="96" spans="8:9">
+      <c r="H96" s="16"/>
+    </row>
+    <row r="97" spans="8:9">
+      <c r="I97" s="16"/>
+    </row>
+    <row r="98" spans="8:9">
+      <c r="H98" s="16"/>
+    </row>
+    <row r="99" spans="8:9">
+      <c r="H99" s="16"/>
+    </row>
+    <row r="100" spans="8:9">
+      <c r="H100" s="16"/>
+    </row>
+    <row r="101" spans="8:9">
+      <c r="I101" s="16"/>
+    </row>
+    <row r="102" spans="8:9">
+      <c r="H102" s="16"/>
+    </row>
+    <row r="103" spans="8:9">
+      <c r="H103" s="16"/>
+    </row>
+    <row r="104" spans="8:9">
+      <c r="H104" s="16"/>
+    </row>
+    <row r="105" spans="8:9">
+      <c r="I105" s="16"/>
+    </row>
+    <row r="106" spans="8:9">
+      <c r="H106" s="16"/>
+      <c r="I106" s="16"/>
+    </row>
+    <row r="107" spans="8:9">
+      <c r="H107" s="16"/>
+      <c r="I107" s="16"/>
+    </row>
+    <row r="108" spans="8:9">
+      <c r="H108" s="16"/>
+    </row>
+    <row r="109" spans="8:9">
+      <c r="H109" s="16"/>
+    </row>
+    <row r="110" spans="8:9">
+      <c r="H110" s="16"/>
+    </row>
+    <row r="111" spans="8:9">
+      <c r="H111" s="16"/>
+    </row>
+    <row r="112" spans="8:9">
+      <c r="H112" s="16"/>
+      <c r="I112" s="16"/>
+    </row>
+    <row r="113" spans="8:9">
+      <c r="H113" s="16"/>
+      <c r="I113" s="16"/>
+    </row>
+    <row r="114" spans="8:9">
+      <c r="H114" s="16"/>
+    </row>
+    <row r="115" spans="8:9">
+      <c r="H115" s="16"/>
+    </row>
+    <row r="116" spans="8:9">
+      <c r="H116" s="16"/>
+    </row>
+    <row r="117" spans="8:9">
+      <c r="H117" s="16"/>
+    </row>
+    <row r="118" spans="8:9">
+      <c r="H118" s="16"/>
+    </row>
+    <row r="119" spans="8:9">
+      <c r="I119" s="16"/>
+    </row>
+    <row r="120" spans="8:9">
+      <c r="H120" s="16"/>
+    </row>
+    <row r="121" spans="8:9">
+      <c r="H121" s="16"/>
+    </row>
+    <row r="122" spans="8:9">
+      <c r="I122" s="16"/>
+    </row>
+    <row r="123" spans="8:9">
+      <c r="H123" s="16"/>
+    </row>
+    <row r="124" spans="8:9">
+      <c r="H124" s="16"/>
+    </row>
+    <row r="125" spans="8:9">
+      <c r="H125" s="16"/>
+    </row>
+    <row r="126" spans="8:9">
+      <c r="I126" s="16"/>
+    </row>
+    <row r="127" spans="8:9">
+      <c r="I127" s="16"/>
+    </row>
+    <row r="128" spans="8:9">
+      <c r="I128" s="16"/>
+    </row>
+    <row r="129" spans="8:9">
+      <c r="H129" s="16"/>
+    </row>
+    <row r="130" spans="8:9">
+      <c r="H130" s="16"/>
+      <c r="I130" s="16"/>
+    </row>
+    <row r="131" spans="8:9">
+      <c r="H131" s="16"/>
+    </row>
+    <row r="132" spans="8:9">
+      <c r="H132" s="16"/>
+    </row>
+    <row r="133" spans="8:9">
+      <c r="H133" s="16"/>
+    </row>
+    <row r="134" spans="8:9">
+      <c r="H134" s="16"/>
+    </row>
+    <row r="135" spans="8:9">
+      <c r="H135" s="16"/>
+      <c r="I135" s="16"/>
+    </row>
+    <row r="136" spans="8:9">
+      <c r="I136" s="16"/>
+    </row>
+    <row r="137" spans="8:9">
+      <c r="H137" s="16"/>
+    </row>
+    <row r="138" spans="8:9">
+      <c r="H138" s="16"/>
+      <c r="I138" s="16"/>
+    </row>
+    <row r="139" spans="8:9">
+      <c r="H139" s="16"/>
+    </row>
+    <row r="140" spans="8:9">
+      <c r="I140" s="16"/>
+    </row>
+    <row r="141" spans="8:9">
+      <c r="H141" s="16"/>
+    </row>
+    <row r="142" spans="8:9">
+      <c r="I142" s="16"/>
+    </row>
+    <row r="143" spans="8:9">
+      <c r="I143" s="16"/>
+    </row>
+    <row r="144" spans="8:9">
+      <c r="I144" s="16"/>
+    </row>
+    <row r="145" spans="8:9">
+      <c r="I145" s="16"/>
+    </row>
+    <row r="146" spans="8:9">
+      <c r="H146" s="16"/>
+    </row>
+    <row r="147" spans="8:9">
+      <c r="H147" s="16"/>
+    </row>
+    <row r="148" spans="8:9">
+      <c r="H148" s="16"/>
+      <c r="I148" s="16"/>
+    </row>
+    <row r="149" spans="8:9">
+      <c r="H149" s="16"/>
+    </row>
+    <row r="150" spans="8:9">
+      <c r="H150" s="16"/>
+    </row>
+    <row r="151" spans="8:9">
+      <c r="H151" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37403,7 +37711,7 @@
         <v>0.1968</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="I2" s="16"/>
     </row>
@@ -37415,7 +37723,7 @@
         <v>0.10720000000000002</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="H3" s="16"/>
     </row>
@@ -37427,7 +37735,7 @@
         <v>0.17320000000000002</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="H4" s="16"/>
     </row>
@@ -38357,16 +38665,16 @@
         <v>735</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="K1" s="16" t="s">
         <v>4</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="M1" s="16" t="s">
         <v>771</v>
@@ -38380,10 +38688,10 @@
         <v>736</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="K2" s="16" t="s">
         <v>84</v>
@@ -38397,7 +38705,7 @@
         <v>737</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K3" s="16" t="s">
         <v>92</v>
@@ -38411,7 +38719,7 @@
         <v>738</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>96</v>
@@ -38425,7 +38733,7 @@
         <v>739</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>99</v>
@@ -38445,7 +38753,7 @@
         <v>740</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>103</v>
@@ -38465,7 +38773,7 @@
         <v>741</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>106</v>
@@ -38485,7 +38793,7 @@
         <v>742</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K8" s="16" t="s">
         <v>109</v>
@@ -38505,7 +38813,7 @@
         <v>289</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>112</v>
@@ -38519,7 +38827,7 @@
         <v>743</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>115</v>
@@ -38539,7 +38847,7 @@
         <v>744</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>118</v>
@@ -38559,7 +38867,7 @@
         <v>745</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>121</v>
@@ -38579,7 +38887,7 @@
         <v>746</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>121</v>
@@ -38599,7 +38907,7 @@
         <v>747</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>126</v>
@@ -38619,7 +38927,7 @@
         <v>748</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K15" s="16" t="s">
         <v>131</v>
@@ -38633,7 +38941,7 @@
         <v>749</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>135</v>
@@ -38653,7 +38961,7 @@
         <v>750</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K17" s="16" t="s">
         <v>138</v>
@@ -38673,7 +38981,7 @@
         <v>751</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>142</v>
@@ -38693,7 +39001,7 @@
         <v>752</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K19" s="16" t="s">
         <v>146</v>
@@ -38713,7 +39021,7 @@
         <v>753</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K20" s="16" t="s">
         <v>150</v>
@@ -38733,7 +39041,7 @@
         <v>754</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>150</v>
@@ -38753,7 +39061,7 @@
         <v>459</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>154</v>
@@ -38767,7 +39075,7 @@
         <v>336</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>159</v>
@@ -38979,7 +39287,7 @@
         <v>135</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K36" s="16" t="s">
         <v>207</v>
@@ -39483,13 +39791,13 @@
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="14" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B63" s="12" t="s">
         <v>150</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="K63" s="16" t="s">
         <v>297</v>
@@ -39503,7 +39811,7 @@
         <v>324</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="K64" s="16" t="s">
         <v>300</v>

</xml_diff>